<commit_message>
Projeto Completo com SEO e Documentação - React em Anexo
</commit_message>
<xml_diff>
--- a/SEO/Plano de SEO.xlsx
+++ b/SEO/Plano de SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive (Vitor Tomazi)\Google Drive (Vitor Tomazi)\Computação Estudo\Admissão 2BChosen Vitor Tomazi\SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AC3314-CDB0-45FF-B2D2-32BFB394497E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B6761E-E0E7-45F0-8D22-304139A09B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="700" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="700" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquitetura" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="170">
   <si>
     <t>Mês/Métrica</t>
   </si>
@@ -434,12 +434,6 @@
     <t>Não disponível ainda para o mercado</t>
   </si>
   <si>
-    <t>A ser definido</t>
-  </si>
-  <si>
-    <t>A ser difinido (Index curso de culinária)</t>
-  </si>
-  <si>
     <t>Esta planilha é utilizada para monitorar os resultados APÓS o lançamento do site. Por ora a mesma está propositalmente sem dados.</t>
   </si>
   <si>
@@ -528,6 +522,33 @@
   </si>
   <si>
     <t>https://www.2bchosenexemple.com.br/curso-de-culinaria-para-iniciantes</t>
+  </si>
+  <si>
+    <t>Esta aba se refere a futuras parcerias afim de ganhar links/indicações</t>
+  </si>
+  <si>
+    <t>https://www.2bchosenculinary.com.br</t>
+  </si>
+  <si>
+    <t>fácil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sem dado do Adwords </t>
+  </si>
+  <si>
+    <t>É uma home page</t>
+  </si>
+  <si>
+    <t>não (é um Lorem ipsum)</t>
+  </si>
+  <si>
+    <t>é uma home page</t>
+  </si>
+  <si>
+    <t>cursos</t>
+  </si>
+  <si>
+    <t>curso de culinária para iniciantes</t>
   </si>
 </sst>
 </file>
@@ -825,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -882,20 +903,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -903,12 +911,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -937,6 +941,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1264,363 +1291,363 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="97.140625" style="59" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="59" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="59" customWidth="1"/>
-    <col min="4" max="4" width="86.85546875" style="59" customWidth="1"/>
-    <col min="5" max="16384" width="14.42578125" style="59"/>
+    <col min="1" max="1" width="97.140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="50" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="50" customWidth="1"/>
+    <col min="4" max="4" width="86.85546875" style="50" customWidth="1"/>
+    <col min="5" max="16384" width="14.42578125" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="56" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="52" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="52" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="62"/>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="60"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="53"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="53"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="62"/>
+      <c r="D9" s="53"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="62"/>
+      <c r="D10" s="53"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="62"/>
+      <c r="D11" s="53"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="62"/>
+      <c r="D12" s="53"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="51" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="62"/>
+      <c r="D14" s="53"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="52" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="52" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="62"/>
+      <c r="D17" s="53"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="62"/>
+      <c r="D18" s="53"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="62"/>
+      <c r="D19" s="53"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="62"/>
+      <c r="D20" s="53"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="62"/>
+      <c r="D21" s="53"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="62"/>
+      <c r="D22" s="53"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="62"/>
+      <c r="D23" s="53"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="62" t="s">
+      <c r="A24" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="62"/>
+      <c r="D24" s="53"/>
     </row>
     <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="62"/>
+      <c r="D25" s="53"/>
     </row>
     <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="53"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="62"/>
+      <c r="D27" s="53"/>
     </row>
     <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="62"/>
+      <c r="D28" s="53"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="62"/>
+      <c r="D29" s="53"/>
     </row>
     <row r="30" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="63"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="62"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1634,8 +1661,8 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1652,52 +1679,52 @@
       <c r="A1" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="69" t="s">
-        <v>147</v>
+      <c r="B3" s="60" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="59">
         <v>590</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="54" t="s">
-        <v>138</v>
+      <c r="A5" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>136</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
@@ -1740,22 +1767,22 @@
         <v>184.31599999999997</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="G8" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="H8" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1770,22 +1797,22 @@
         <v>82.835999999999999</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="F9" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="48" t="s">
         <v>140</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1800,22 +1827,22 @@
         <v>58.115000000000002</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="G10" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="H10" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="I10" s="56" t="s">
-        <v>140</v>
+      <c r="F10" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1830,22 +1857,22 @@
         <v>41.123000000000005</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="F11" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="I11" s="71" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="62" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1859,23 +1886,23 @@
         <f t="shared" si="0"/>
         <v>32.450000000000003</v>
       </c>
-      <c r="D12" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="H12" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="I12" s="56" t="s">
-        <v>160</v>
+      <c r="D12" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1890,22 +1917,22 @@
         <v>22.006999999999998</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="E13" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="G13" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="H13" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="I13" s="56" t="s">
-        <v>140</v>
+        <v>150</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1920,22 +1947,22 @@
         <v>22.006999999999998</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="F14" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="G14" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="H14" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="I14" s="56" t="s">
-        <v>140</v>
+        <v>151</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1950,22 +1977,22 @@
         <v>22.006999999999998</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="F15" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="G15" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="H15" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="I15" s="56" t="s">
-        <v>140</v>
+        <v>152</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1980,22 +2007,22 @@
         <v>22.006999999999998</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="F16" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="G16" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="H16" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="I16" s="56" t="s">
-        <v>140</v>
+        <v>154</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2010,49 +2037,49 @@
         <v>22.006999999999998</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="F17" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="G17" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="H17" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="H17" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="I17" s="48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="I17" s="56" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
-        <v>161</v>
-      </c>
-      <c r="D19" s="72" t="s">
-        <v>162</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="G19" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="H19" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="I19" s="56" t="s">
-        <v>140</v>
+      <c r="D19" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="H19" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="52"/>
+      <c r="D21" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2076,7 +2103,7 @@
   <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2103,7 +2130,9 @@
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="C2" s="75" t="s">
+        <v>145</v>
+      </c>
       <c r="D2" s="19"/>
       <c r="E2" s="20" t="s">
         <v>54</v>
@@ -2140,9 +2169,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="76" t="s">
+        <v>168</v>
+      </c>
       <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="C5" s="75" t="s">
+        <v>169</v>
+      </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
         <v>83</v>
@@ -2954,7 +2987,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2966,12 +2999,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27"/>
@@ -2994,11 +3027,15 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="33">
+        <v>590</v>
+      </c>
+      <c r="C4" s="35">
+        <v>21</v>
+      </c>
       <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3037,7 +3074,9 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3142,9 +3181,11 @@
   <sheetPr>
     <tabColor rgb="FFFF9900"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3156,65 +3197,62 @@
     <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="72" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B2" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
@@ -3224,6 +3262,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
@@ -3237,7 +3276,7 @@
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -3247,14 +3286,26 @@
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3268,7 +3319,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3280,24 +3331,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="A1" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
     </row>
     <row r="2" spans="1:8" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="46"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -3323,21 +3374,21 @@
       <c r="C6" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="51" t="s">
-        <v>131</v>
+      <c r="D6" s="73" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="68"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -3352,18 +3403,18 @@
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
+      <c r="A12" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3372,8 +3423,8 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" display="www.meusite.com.br/produtoa" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A11" r:id="rId2" display="www.meusite.com.br/pg1" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A11" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -3401,18 +3452,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="A1" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -3503,9 +3554,11 @@
   <sheetPr>
     <tabColor rgb="FF0000FF"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3589,6 +3642,65 @@
         <v>78</v>
       </c>
     </row>
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2">
+        <v>590</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" t="s">
+        <v>149</v>
+      </c>
+      <c r="O2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>